<commit_message>
Record transaction hash to batch file
</commit_message>
<xml_diff>
--- a/test/excel.xlsx
+++ b/test/excel.xlsx
@@ -3,18 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gary/gopath/src/github.com/rjl493456442/ethclient/test/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="500"/>
+    <workbookView tabRatio="500" windowHeight="15540" windowWidth="25520" xWindow="-5780" yWindow="-18880"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" relationships:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000" concurrentCalc="false"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>From</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -86,14 +81,18 @@
   </si>
   <si>
     <t>helloworld</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hash</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -112,10 +111,16 @@
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill patternType="none">
+        <fgColor/>
+        <bgColor/>
+      </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="gray125">
+        <fgColor/>
+        <bgColor/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -128,16 +133,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="常规" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7" defaultTableStyle="TableStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -407,90 +412,6 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="47.83203125" customWidth="1"/>
-    <col min="2" max="2" width="50.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
-        <v>100</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3">
-        <v>100</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4">
-        <v>100</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="UTF-8" standalone="yes"?>
+
 </file>
</xml_diff>

<commit_message>
Add macro definition to usage
</commit_message>
<xml_diff>
--- a/test/excel.xlsx
+++ b/test/excel.xlsx
@@ -3,13 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gary/gopath/src/github.com/rjl493456442/ethclient/test/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView tabRatio="500" windowHeight="15540" windowWidth="25520" xWindow="-5780" yWindow="-18880"/>
+    <workbookView xWindow="-12800" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" relationships:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="false"/>
+  <calcPr calcId="150000" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -22,25 +28,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>From</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>To</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Value</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Passphrase</t>
+  </si>
+  <si>
+    <t>0x168f70A4b92E630b31Ab887Fb7956ddB7C3813cf</t>
+  </si>
+  <si>
+    <t>0x0</t>
+  </si>
+  <si>
+    <t>0x65F28650F3c9721580b81c6d552999270EffFCb1</t>
+  </si>
+  <si>
+    <t>0x2C77c0eb01005f8abca57C7c94732A642F825bd8</t>
+  </si>
+  <si>
+    <t>hello world</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -48,51 +65,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0x168f70A4b92E630b31Ab887Fb7956ddB7C3813cf</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x123456</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>helloworld</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>0x7Cd6342b4b02A90bcf60F1f843d1002897e38b1f</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0x65F28650F3c9721580b81c6d552999270EffFCb1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>0xfFc1736f670f305A3d752280d07F6895379cbD70</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x2C77c0eb01005f8abca57C7c94732A642F825bd8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x123456</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>helloworld</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hash</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -108,19 +93,21 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="DengXian"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none">
-        <fgColor/>
-        <bgColor/>
-      </patternFill>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor/>
-        <bgColor/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -133,16 +120,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="常规" xfId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -412,6 +401,90 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="UTF-8" standalone="yes"?>
-
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="60.1640625" customWidth="1"/>
+    <col min="2" max="2" width="51.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2">
+        <v>10000000000000</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1">
+        <v>10000000000</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1000000000000</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>